<commit_message>
include mu in the CS kernel xlsx
</commit_message>
<xml_diff>
--- a/cskernel.xlsx
+++ b/cskernel.xlsx
@@ -5,34 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barryp/work/JAM/fitpack2/database/CS_kernel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/barryp/work/JAM/fitpack2/database/CS_kernel/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3520CF0D-4461-5647-9266-4FF2A78C65B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A9E64C-3D27-8C4E-80FE-5E488357490C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33020" yWindow="5420" windowWidth="34120" windowHeight="13440" xr2:uid="{C7D89C0D-F0E8-AB49-A7F4-CE0E323DCFFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$2:$A$8</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$2:$B$8</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
   <si>
     <t>bT</t>
   </si>
@@ -80,12 +63,18 @@
   </si>
   <si>
     <t>Msbar, uNNLL, bT in GeV^-1</t>
+  </si>
+  <si>
+    <t>mu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -121,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,179 +427,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A998C6B2-44AE-0740-A276-5002B0FC8740}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>0.12*5.068</f>
         <v>0.60815999999999992</v>
       </c>
-      <c r="B2">
-        <v>0.12</v>
+      <c r="B2" s="1">
+        <v>2</v>
       </c>
       <c r="C2">
         <v>0.12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>0.12</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>0.24*5.068</f>
         <v>1.2163199999999998</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>-0.2</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.09</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <f>0.36*5.068</f>
         <v>1.8244799999999999</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4">
         <v>-0.43</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <f>0.48*5.068</f>
         <v>2.4326399999999997</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5">
         <v>-0.64</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>0.6*5.068</f>
         <v>3.0407999999999995</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6">
         <v>-0.8</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <f>0.72*5.068</f>
         <v>3.6489599999999998</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7">
         <v>-0.94</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.41</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <f>0.84*5.068</f>
         <v>4.2571199999999996</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8">
         <v>-1.24</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.68</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>